<commit_message>
fix: build passes locally; ensure file paths & env
</commit_message>
<xml_diff>
--- a/PO_test/PO_Excel_InputSheet_Template_updated.xlsx
+++ b/PO_test/PO_Excel_InputSheet_Template_updated.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidyang/workspace/20250713_PO_Mgmt/PO_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902059DD-D14B-714E-A095-F8A02554A1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A917A9-355B-A446-B4AE-D04760A30DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="2260" windowWidth="33400" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5960" yWindow="2260" windowWidth="27340" windowHeight="13240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -137,8 +150,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="_-[$₩-412]* #,##0_-;\-[$₩-412]* #,##0_-;_-[$₩-412]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="#,##0_ "/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -205,13 +220,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -517,7 +534,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -525,7 +542,9 @@
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="12" customWidth="1"/>
     <col min="11" max="11" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="12" customWidth="1"/>
+    <col min="12" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -611,14 +630,15 @@
         <v>24</v>
       </c>
       <c r="L2" s="3"/>
-      <c r="M2" s="3">
+      <c r="M2" s="5">
         <v>2025.1475700000001</v>
       </c>
-      <c r="N2" s="3">
-        <v>6150</v>
-      </c>
-      <c r="O2" s="3">
-        <v>12454657.555500001</v>
+      <c r="N2" s="4">
+        <v>400</v>
+      </c>
+      <c r="O2" s="4">
+        <f>M2*N2</f>
+        <v>810059.02800000005</v>
       </c>
       <c r="P2" s="3"/>
     </row>
@@ -655,14 +675,15 @@
         <v>30</v>
       </c>
       <c r="L3" s="3"/>
-      <c r="M3" s="3">
+      <c r="M3" s="5">
         <v>1739.6189199999999</v>
       </c>
-      <c r="N3" s="3">
-        <v>6200</v>
-      </c>
-      <c r="O3" s="3">
-        <v>10785637.304</v>
+      <c r="N3" s="4">
+        <v>300</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" ref="O3:O4" si="0">M3*N3</f>
+        <v>521885.67599999998</v>
       </c>
       <c r="P3" s="3"/>
     </row>
@@ -699,14 +720,15 @@
         <v>36</v>
       </c>
       <c r="L4" s="3"/>
-      <c r="M4" s="3">
+      <c r="M4" s="5">
         <v>366.24</v>
       </c>
-      <c r="N4" s="3">
-        <v>8500</v>
-      </c>
-      <c r="O4" s="3">
-        <v>3113040</v>
+      <c r="N4" s="4">
+        <v>200</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="0"/>
+        <v>73248</v>
       </c>
       <c r="P4" s="3"/>
     </row>

</xml_diff>